<commit_message>
attempt at new linear multibracket framing
</commit_message>
<xml_diff>
--- a/thesis-tex/todo.xlsx
+++ b/thesis-tex/todo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4ECAB17-5447-4BBF-A5DE-830B1E11935F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E683F033-0900-4D59-B81C-BCB2DBE0F343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{5E98CAFA-3C68-43D4-B8FA-5BDF0312E4FD}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="65">
   <si>
     <t>Graphics</t>
   </si>
@@ -228,6 +229,9 @@
   </si>
   <si>
     <t>nlf 2024</t>
+  </si>
+  <si>
+    <t>THE NETWORK CONDITION</t>
   </si>
 </sst>
 </file>
@@ -630,29 +634,31 @@
   <dimension ref="B3:M69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="48.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.21875" customWidth="1"/>
-    <col min="9" max="9" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" customWidth="1"/>
+    <col min="9" max="9" width="28.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="I3" s="6"/>
-      <c r="K3" s="6"/>
+      <c r="K3" s="7" t="s">
+        <v>64</v>
+      </c>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
         <v>0</v>
       </c>
@@ -675,7 +681,7 @@
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -707,7 +713,7 @@
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>12</v>
       </c>
@@ -739,7 +745,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>12</v>
       </c>
@@ -771,7 +777,7 @@
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -803,7 +809,7 @@
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>12</v>
       </c>
@@ -833,7 +839,7 @@
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>12</v>
       </c>
@@ -863,7 +869,7 @@
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>12</v>
       </c>
@@ -892,7 +898,7 @@
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -919,7 +925,7 @@
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -946,7 +952,7 @@
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>12</v>
       </c>
@@ -973,7 +979,7 @@
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>12</v>
       </c>
@@ -996,7 +1002,7 @@
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>12</v>
       </c>
@@ -1020,7 +1026,7 @@
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>12</v>
       </c>
@@ -1037,7 +1043,7 @@
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>12</v>
       </c>
@@ -1054,7 +1060,7 @@
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>12</v>
       </c>
@@ -1074,7 +1080,7 @@
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>12</v>
       </c>
@@ -1093,7 +1099,7 @@
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>12</v>
       </c>
@@ -1112,7 +1118,7 @@
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>12</v>
       </c>
@@ -1131,7 +1137,7 @@
       <c r="L22" s="8"/>
       <c r="M22" s="8"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>12</v>
       </c>
@@ -1150,7 +1156,7 @@
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>12</v>
       </c>
@@ -1169,7 +1175,7 @@
       <c r="L24" s="8"/>
       <c r="M24" s="8"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>12</v>
       </c>
@@ -1188,7 +1194,7 @@
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>12</v>
       </c>
@@ -1197,7 +1203,7 @@
       <c r="L26" s="8"/>
       <c r="M26" s="8"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>12</v>
       </c>
@@ -1205,7 +1211,7 @@
       <c r="L27" s="8"/>
       <c r="M27" s="8"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>12</v>
       </c>
@@ -1213,7 +1219,7 @@
       <c r="L28" s="8"/>
       <c r="M28" s="8"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>12</v>
       </c>
@@ -1221,202 +1227,202 @@
       <c r="L29" s="8"/>
       <c r="M29" s="8"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
linear multibrackets with semibrackets in the middle
</commit_message>
<xml_diff>
--- a/thesis-tex/todo.xlsx
+++ b/thesis-tex/todo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E683F033-0900-4D59-B81C-BCB2DBE0F343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6113ADB6-26BD-4482-8ED8-6EE4C88CEEA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{5E98CAFA-3C68-43D4-B8FA-5BDF0312E4FD}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="66">
   <si>
     <t>Graphics</t>
   </si>
@@ -232,6 +232,9 @@
   </si>
   <si>
     <t>THE NETWORK CONDITION</t>
+  </si>
+  <si>
+    <t>itermize vs enumberate</t>
   </si>
 </sst>
 </file>
@@ -634,7 +637,7 @@
   <dimension ref="B3:M69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,7 +994,9 @@
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="G15" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="H15" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
lost some of bracket.xlsx
</commit_message>
<xml_diff>
--- a/thesis-tex/todo.xlsx
+++ b/thesis-tex/todo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6113ADB6-26BD-4482-8ED8-6EE4C88CEEA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA17858C-5FB1-476F-B830-2CDBF3D0D1A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{5E98CAFA-3C68-43D4-B8FA-5BDF0312E4FD}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="67">
   <si>
     <t>Graphics</t>
   </si>
@@ -235,6 +234,9 @@
   </si>
   <si>
     <t>itermize vs enumberate</t>
+  </si>
+  <si>
+    <t>empty tournament is not one</t>
   </si>
 </sst>
 </file>
@@ -637,18 +639,18 @@
   <dimension ref="B3:M69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="48.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.28515625" customWidth="1"/>
-    <col min="9" max="9" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.33203125" customWidth="1"/>
+    <col min="9" max="9" width="28.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -661,7 +663,7 @@
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C4" s="5" t="s">
         <v>0</v>
       </c>
@@ -684,7 +686,7 @@
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -716,7 +718,7 @@
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>12</v>
       </c>
@@ -748,7 +750,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>12</v>
       </c>
@@ -780,7 +782,7 @@
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -812,7 +814,7 @@
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>12</v>
       </c>
@@ -842,7 +844,7 @@
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>12</v>
       </c>
@@ -872,7 +874,7 @@
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>12</v>
       </c>
@@ -901,7 +903,7 @@
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -928,7 +930,7 @@
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -955,7 +957,7 @@
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>12</v>
       </c>
@@ -982,7 +984,7 @@
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>12</v>
       </c>
@@ -1003,11 +1005,13 @@
       <c r="J15" t="s">
         <v>12</v>
       </c>
-      <c r="K15" s="8"/>
+      <c r="K15" s="8" t="s">
+        <v>66</v>
+      </c>
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>12</v>
       </c>
@@ -1031,7 +1035,7 @@
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>12</v>
       </c>
@@ -1048,7 +1052,7 @@
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>12</v>
       </c>
@@ -1065,7 +1069,7 @@
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>12</v>
       </c>
@@ -1085,7 +1089,7 @@
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>12</v>
       </c>
@@ -1104,7 +1108,7 @@
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>12</v>
       </c>
@@ -1123,7 +1127,7 @@
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>12</v>
       </c>
@@ -1142,7 +1146,7 @@
       <c r="L22" s="8"/>
       <c r="M22" s="8"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>12</v>
       </c>
@@ -1161,7 +1165,7 @@
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>12</v>
       </c>
@@ -1180,7 +1184,7 @@
       <c r="L24" s="8"/>
       <c r="M24" s="8"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>12</v>
       </c>
@@ -1199,7 +1203,7 @@
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>12</v>
       </c>
@@ -1208,7 +1212,7 @@
       <c r="L26" s="8"/>
       <c r="M26" s="8"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>12</v>
       </c>
@@ -1216,7 +1220,7 @@
       <c r="L27" s="8"/>
       <c r="M27" s="8"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>12</v>
       </c>
@@ -1224,7 +1228,7 @@
       <c r="L28" s="8"/>
       <c r="M28" s="8"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>12</v>
       </c>
@@ -1232,202 +1236,202 @@
       <c r="L29" s="8"/>
       <c r="M29" s="8"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>12</v>
       </c>

</xml_diff>